<commit_message>
Scripts update and new/updated input files
</commit_message>
<xml_diff>
--- a/input_data/Manuscript_4_data.xlsx
+++ b/input_data/Manuscript_4_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rita\Documents\R\Manuscript_4\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rita\Documents\R\amendment_micropollutant_biodegradation_aquifer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1564AE-86B0-4767-83D4-3ABFFF991EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3366867-B761-4C68-9BC7-89378A1F5939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7700" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7721" uniqueCount="55">
   <si>
     <t>NA</t>
   </si>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7327B6D-C7AD-4AA7-BC22-6EE4F3094F03}">
   <dimension ref="A1:AN465"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="Q250" workbookViewId="0">
+      <selection activeCell="AE261" sqref="AE261:AE266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -965,50 +965,50 @@
       <c r="R4" t="s">
         <v>0</v>
       </c>
-      <c r="S4" s="2">
-        <v>3.3868974042027191</v>
-      </c>
-      <c r="T4" s="2">
-        <v>2.6126614987080101</v>
-      </c>
-      <c r="U4" s="2">
-        <v>4.2931937172774868</v>
-      </c>
-      <c r="V4" s="2">
-        <v>3.7814063563365723</v>
-      </c>
-      <c r="W4" s="2">
-        <v>3.3644859813084116</v>
-      </c>
-      <c r="X4" s="2">
-        <v>3.0608631313803065</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>3.3322636461845119</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>3.7753036437246958</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>3.9618347542471652</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>4.1997197969693936</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>3.5182708473716313</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>3.6990465686981846</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>3.6333699231613616</v>
-      </c>
-      <c r="AF4" s="2">
-        <v>4.830421377183967</v>
-      </c>
-      <c r="AG4" s="2">
-        <v>4.6432264736297828</v>
+      <c r="S4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AH4" s="2" t="s">
         <v>0</v>
@@ -4732,10 +4732,10 @@
       <c r="M35">
         <v>0.44</v>
       </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
+      <c r="N35" s="2">
+        <v>0</v>
+      </c>
+      <c r="O35" s="2">
         <v>0</v>
       </c>
       <c r="P35">
@@ -4854,10 +4854,10 @@
       <c r="M36">
         <v>0.34100000000000008</v>
       </c>
-      <c r="N36">
-        <v>0.46700000000000014</v>
-      </c>
-      <c r="O36">
+      <c r="N36" s="2">
+        <v>0.42454545454545473</v>
+      </c>
+      <c r="O36" s="2">
         <v>0</v>
       </c>
       <c r="P36">
@@ -4976,10 +4976,10 @@
       <c r="M37">
         <v>0.36399999999999999</v>
       </c>
-      <c r="N37">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="O37">
+      <c r="N37" s="2">
+        <v>0.75545454545454538</v>
+      </c>
+      <c r="O37" s="2">
         <v>0</v>
       </c>
       <c r="P37">
@@ -5098,10 +5098,10 @@
       <c r="M38">
         <v>0.33800000000000002</v>
       </c>
-      <c r="N38">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="O38">
+      <c r="N38" s="2">
+        <v>0.43181818181818182</v>
+      </c>
+      <c r="O38" s="2">
         <v>0</v>
       </c>
       <c r="P38">
@@ -5220,10 +5220,10 @@
       <c r="M39">
         <v>0.48600000000000004</v>
       </c>
-      <c r="N39">
-        <v>0.86400000000000021</v>
-      </c>
-      <c r="O39">
+      <c r="N39" s="2">
+        <v>0.78545454545454563</v>
+      </c>
+      <c r="O39" s="2">
         <v>0</v>
       </c>
       <c r="P39">
@@ -5342,10 +5342,10 @@
       <c r="M40">
         <v>0.48899999999999999</v>
       </c>
-      <c r="N40">
-        <v>0.86900000000000022</v>
-      </c>
-      <c r="O40">
+      <c r="N40" s="2">
+        <v>0.79000000000000015</v>
+      </c>
+      <c r="O40" s="2">
         <v>0</v>
       </c>
       <c r="P40">
@@ -14614,11 +14614,11 @@
       <c r="M116">
         <v>0.47499999999999998</v>
       </c>
-      <c r="N116">
-        <v>1.27</v>
-      </c>
-      <c r="O116">
-        <v>0.12</v>
+      <c r="N116" s="2">
+        <v>1.1545454545454545</v>
+      </c>
+      <c r="O116" s="2">
+        <v>4.5454545454546302E-3</v>
       </c>
       <c r="P116">
         <v>1.1499999999999999</v>
@@ -14736,11 +14736,11 @@
       <c r="M117">
         <v>2.67</v>
       </c>
-      <c r="N117">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="O117">
-        <v>4.26</v>
+      <c r="N117" s="2">
+        <v>30.27272727272727</v>
+      </c>
+      <c r="O117" s="2">
+        <v>1.1727272727272684</v>
       </c>
       <c r="P117">
         <v>29.1</v>
@@ -14858,10 +14858,10 @@
       <c r="M118">
         <v>0.27900000000000003</v>
       </c>
-      <c r="N118">
-        <v>5.43</v>
-      </c>
-      <c r="O118">
+      <c r="N118" s="2">
+        <v>4.9363636363636365</v>
+      </c>
+      <c r="O118" s="2">
         <v>0</v>
       </c>
       <c r="P118">
@@ -14980,11 +14980,11 @@
       <c r="M119">
         <v>0.33100000000000007</v>
       </c>
-      <c r="N119">
-        <v>6.1</v>
-      </c>
-      <c r="O119">
-        <v>0.19</v>
+      <c r="N119" s="2">
+        <v>5.5454545454545459</v>
+      </c>
+      <c r="O119" s="2">
+        <v>0</v>
       </c>
       <c r="P119">
         <v>5.91</v>
@@ -15102,11 +15102,11 @@
       <c r="M120">
         <v>0.35700000000000004</v>
       </c>
-      <c r="N120">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="O120">
-        <v>0.55000000000000004</v>
+      <c r="N120" s="2">
+        <v>7.6818181818181808</v>
+      </c>
+      <c r="O120" s="2">
+        <v>0</v>
       </c>
       <c r="P120">
         <v>7.9</v>
@@ -15224,11 +15224,11 @@
       <c r="M121">
         <v>0.28399999999999997</v>
       </c>
-      <c r="N121">
-        <v>8.56</v>
-      </c>
-      <c r="O121">
-        <v>0.59</v>
+      <c r="N121" s="2">
+        <v>7.7818181818181822</v>
+      </c>
+      <c r="O121" s="2">
+        <v>0</v>
       </c>
       <c r="P121">
         <v>7.97</v>
@@ -26937,7 +26937,7 @@
         <v>0.46600000000000008</v>
       </c>
       <c r="N217">
-        <v>0.48100000000000004</v>
+        <v>0.43727272727272731</v>
       </c>
       <c r="O217">
         <v>0</v>
@@ -27059,10 +27059,10 @@
         <v>3.65</v>
       </c>
       <c r="N218">
-        <v>21.9</v>
+        <v>19.90909090909091</v>
       </c>
       <c r="O218">
-        <v>1.81</v>
+        <v>0</v>
       </c>
       <c r="P218">
         <v>20.100000000000001</v>
@@ -27181,10 +27181,10 @@
         <v>0.44700000000000012</v>
       </c>
       <c r="N219">
-        <v>4.4000000000000004</v>
+        <v>4.0000000000000009</v>
       </c>
       <c r="O219">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="P219">
         <v>4.1500000000000004</v>
@@ -27303,10 +27303,10 @@
         <v>0.12400000000000001</v>
       </c>
       <c r="N220">
-        <v>6.19</v>
+        <v>5.627272727272727</v>
       </c>
       <c r="O220">
-        <v>0.71</v>
+        <v>0</v>
       </c>
       <c r="P220">
         <v>5.48</v>
@@ -27425,10 +27425,10 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="N221">
-        <v>12.1</v>
+        <v>11</v>
       </c>
       <c r="O221">
-        <v>1.0900000000000001</v>
+        <v>0</v>
       </c>
       <c r="P221">
         <v>11</v>
@@ -27547,10 +27547,10 @@
         <v>0.46400000000000002</v>
       </c>
       <c r="N222">
-        <v>8.7799999999999994</v>
+        <v>7.9818181818181806</v>
       </c>
       <c r="O222">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P222">
         <v>8.2799999999999994</v>
@@ -32355,8 +32355,8 @@
       <c r="AD261" s="2">
         <v>1</v>
       </c>
-      <c r="AE261" s="2">
-        <v>1</v>
+      <c r="AE261" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AF261" s="2">
         <v>1</v>
@@ -32477,7 +32477,7 @@
       <c r="AD262" s="2">
         <v>0.88642910490356719</v>
       </c>
-      <c r="AE262" s="2">
+      <c r="AE262" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AF262" s="2">
@@ -32599,7 +32599,7 @@
       <c r="AD263" s="2">
         <v>0.96204242730047873</v>
       </c>
-      <c r="AE263" s="2">
+      <c r="AE263" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AF263" s="2">
@@ -32721,7 +32721,7 @@
       <c r="AD264" s="2">
         <v>0.99753858751969693</v>
       </c>
-      <c r="AE264" s="2">
+      <c r="AE264" s="2" t="s">
         <v>0</v>
       </c>
       <c r="AF264" s="2">
@@ -32843,8 +32843,8 @@
       <c r="AD265" s="2">
         <v>0.9775495271552368</v>
       </c>
-      <c r="AE265" s="2">
-        <v>0.33429484768401774</v>
+      <c r="AE265" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AF265" s="2">
         <v>1.0084745762711864</v>
@@ -32965,8 +32965,8 @@
       <c r="AD266" s="2">
         <v>1.1359620450748666</v>
       </c>
-      <c r="AE266" s="2">
-        <v>0.38421640696906534</v>
+      <c r="AE266" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="AF266" s="2">
         <v>1.0932203389830508</v>
@@ -44383,7 +44383,7 @@
         <v>0.35899999999999999</v>
       </c>
       <c r="N360">
-        <v>0.51400000000000001</v>
+        <v>0.46727272727272728</v>
       </c>
       <c r="O360">
         <v>0</v>
@@ -44505,10 +44505,10 @@
         <v>0.58299999999999996</v>
       </c>
       <c r="N361">
-        <v>15.8</v>
+        <v>14.363636363636363</v>
       </c>
       <c r="O361">
-        <v>1.77</v>
+        <v>0</v>
       </c>
       <c r="P361">
         <v>14.1</v>
@@ -44627,10 +44627,10 @@
         <v>0.59499999999999997</v>
       </c>
       <c r="N362">
-        <v>8.8800000000000008</v>
+        <v>8.0727272727272741</v>
       </c>
       <c r="O362">
-        <v>0.69</v>
+        <v>0</v>
       </c>
       <c r="P362">
         <v>8.19</v>
@@ -44749,10 +44749,10 @@
         <v>0.45</v>
       </c>
       <c r="N363">
-        <v>7.43</v>
+        <v>6.7545454545454549</v>
       </c>
       <c r="O363">
-        <v>0.61</v>
+        <v>0</v>
       </c>
       <c r="P363">
         <v>6.82</v>
@@ -44871,7 +44871,7 @@
         <v>0.38700000000000007</v>
       </c>
       <c r="N364">
-        <v>5.66</v>
+        <v>5.1454545454545455</v>
       </c>
       <c r="O364">
         <v>0</v>
@@ -44993,10 +44993,10 @@
         <v>0.35299999999999998</v>
       </c>
       <c r="N365">
-        <v>6.04</v>
+        <v>5.4909090909090912</v>
       </c>
       <c r="O365">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P365">
         <v>5.94</v>
@@ -49263,10 +49263,10 @@
         <v>0.59200000000000008</v>
       </c>
       <c r="N400">
-        <v>3.33</v>
+        <v>3.0272727272727273</v>
       </c>
       <c r="O400">
-        <v>1.44</v>
+        <v>1.1372727272727274</v>
       </c>
       <c r="P400">
         <v>1.89</v>
@@ -49385,10 +49385,10 @@
         <v>0.52300000000000002</v>
       </c>
       <c r="N401">
-        <v>2.97</v>
+        <v>2.7</v>
       </c>
       <c r="O401">
-        <v>1.21</v>
+        <v>0.95000000000000018</v>
       </c>
       <c r="P401">
         <v>1.75</v>
@@ -49507,10 +49507,10 @@
         <v>0.49100000000000005</v>
       </c>
       <c r="N402">
-        <v>2.7</v>
+        <v>2.4545454545454546</v>
       </c>
       <c r="O402">
-        <v>1.05</v>
+        <v>0.80454545454545467</v>
       </c>
       <c r="P402">
         <v>1.65</v>
@@ -49629,10 +49629,10 @@
         <v>11.3</v>
       </c>
       <c r="N403">
-        <v>17.600000000000001</v>
+        <v>16.000000000000004</v>
       </c>
       <c r="O403">
-        <v>3.54</v>
+        <v>2.0000000000000036</v>
       </c>
       <c r="P403">
         <v>14</v>
@@ -49751,10 +49751,10 @@
         <v>0.44600000000000006</v>
       </c>
       <c r="N404">
-        <v>2.44</v>
+        <v>2.2181818181818183</v>
       </c>
       <c r="O404">
-        <v>1.1399999999999999</v>
+        <v>0.91818181818181821</v>
       </c>
       <c r="P404">
         <v>1.3</v>
@@ -49873,10 +49873,10 @@
         <v>0.42799999999999994</v>
       </c>
       <c r="N405">
-        <v>2.3199999999999998</v>
+        <v>2.1090909090909089</v>
       </c>
       <c r="O405">
-        <v>0.875</v>
+        <v>0.65909090909090895</v>
       </c>
       <c r="P405">
         <v>1.45</v>
@@ -49995,10 +49995,10 @@
         <v>0.93300000000000005</v>
       </c>
       <c r="N406">
-        <v>2.36</v>
+        <v>2.1454545454545455</v>
       </c>
       <c r="O406">
-        <v>0.27</v>
+        <v>5.5454545454545645E-2</v>
       </c>
       <c r="P406">
         <v>2.09</v>
@@ -50117,10 +50117,10 @@
         <v>0.70799999999999996</v>
       </c>
       <c r="N407">
-        <v>2.69</v>
+        <v>2.4454545454545453</v>
       </c>
       <c r="O407">
-        <v>0.69799999999999995</v>
+        <v>0.45545454545454533</v>
       </c>
       <c r="P407">
         <v>1.99</v>
@@ -51703,7 +51703,7 @@
         <v>0.623</v>
       </c>
       <c r="N420">
-        <v>2.23</v>
+        <v>2.0272727272727273</v>
       </c>
       <c r="O420">
         <v>0</v>
@@ -51825,10 +51825,10 @@
         <v>40.1</v>
       </c>
       <c r="N421">
-        <v>48.5</v>
+        <v>44.090909090909093</v>
       </c>
       <c r="O421">
-        <v>7.16</v>
+        <v>2.6909090909090949</v>
       </c>
       <c r="P421">
         <v>41.4</v>
@@ -51947,10 +51947,10 @@
         <v>0.52800000000000002</v>
       </c>
       <c r="N422">
-        <v>2.34</v>
+        <v>2.1272727272727274</v>
       </c>
       <c r="O422">
-        <v>0.51900000000000002</v>
+        <v>0.29727272727272736</v>
       </c>
       <c r="P422">
         <v>1.83</v>
@@ -52069,10 +52069,10 @@
         <v>0.52400000000000002</v>
       </c>
       <c r="N423">
-        <v>2.19</v>
+        <v>1.990909090909091</v>
       </c>
       <c r="O423">
-        <v>0.44500000000000001</v>
+        <v>0.24090909090909096</v>
       </c>
       <c r="P423">
         <v>1.75</v>
@@ -52191,10 +52191,10 @@
         <v>0.57700000000000007</v>
       </c>
       <c r="N424">
-        <v>2.36</v>
+        <v>2.1454545454545455</v>
       </c>
       <c r="O424">
-        <v>0.40799999999999997</v>
+        <v>0.19545454545454555</v>
       </c>
       <c r="P424">
         <v>1.95</v>
@@ -52313,10 +52313,10 @@
         <v>0.51400000000000001</v>
       </c>
       <c r="N425">
-        <v>2.1</v>
+        <v>1.9090909090909092</v>
       </c>
       <c r="O425">
-        <v>0.51800000000000002</v>
+        <v>0.31909090909090909</v>
       </c>
       <c r="P425">
         <v>1.59</v>
@@ -52435,10 +52435,10 @@
         <v>0.47399999999999998</v>
       </c>
       <c r="N426">
-        <v>2.09</v>
+        <v>1.9</v>
       </c>
       <c r="O426">
-        <v>0.55300000000000005</v>
+        <v>0.35999999999999988</v>
       </c>
       <c r="P426">
         <v>1.54</v>
@@ -52557,10 +52557,10 @@
         <v>49.4</v>
       </c>
       <c r="N427">
-        <v>59.4</v>
+        <v>54</v>
       </c>
       <c r="O427">
-        <v>8.3800000000000008</v>
+        <v>3</v>
       </c>
       <c r="P427">
         <v>51</v>
@@ -52679,10 +52679,10 @@
         <v>0.504</v>
       </c>
       <c r="N428">
-        <v>2.74</v>
+        <v>2.4909090909090907</v>
       </c>
       <c r="O428">
-        <v>0.80300000000000005</v>
+        <v>0.55090909090909079</v>
       </c>
       <c r="P428">
         <v>1.94</v>
@@ -52801,10 +52801,10 @@
         <v>0.43700000000000011</v>
       </c>
       <c r="N429">
-        <v>2.21</v>
+        <v>2.0090909090909093</v>
       </c>
       <c r="O429">
-        <v>0.58799999999999997</v>
+        <v>0.38909090909090915</v>
       </c>
       <c r="P429">
         <v>1.62</v>
@@ -52923,10 +52923,10 @@
         <v>0.47600000000000003</v>
       </c>
       <c r="N430">
-        <v>2.21</v>
+        <v>2.0090909090909093</v>
       </c>
       <c r="O430">
-        <v>0.57299999999999995</v>
+        <v>0.37909090909090937</v>
       </c>
       <c r="P430">
         <v>1.63</v>
@@ -53045,10 +53045,10 @@
         <v>0.56399999999999995</v>
       </c>
       <c r="N431">
-        <v>2.54</v>
+        <v>2.3090909090909091</v>
       </c>
       <c r="O431">
-        <v>0.875</v>
+        <v>0.64909090909090916</v>
       </c>
       <c r="P431">
         <v>1.66</v>
@@ -56145,6 +56145,7 @@
       <c r="AN465" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AN455" xr:uid="{A7327B6D-C7AD-4AA7-BC22-6EE4F3094F03}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>